<commit_message>
Add improved handlers for workflow, pipeline, and a test harness.
</commit_message>
<xml_diff>
--- a/CreateLotsOfResources/elements.xlsx
+++ b/CreateLotsOfResources/elements.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\code\flow-standalone\electricflow-examples\CreateLotsOfResources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="12315"/>
+    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2967,7 +2972,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3103,7 +3108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3141,6 +3146,9 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3150,6 +3158,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3198,7 +3209,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3231,9 +3242,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3266,6 +3294,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3441,22 +3486,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="140" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="88.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>367</v>
       </c>
       <c r="B1" t="s">
@@ -6467,184 +6511,184 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" tooltip="Symbol (chemistry)" display="https://en.wikipedia.org/wiki/Symbol_(chemistry)"/>
-    <hyperlink ref="C1" r:id="rId2" tooltip="Chemical element" display="https://en.wikipedia.org/wiki/Chemical_element"/>
-    <hyperlink ref="E1" r:id="rId3" tooltip="Group (periodic table)" display="https://en.wikipedia.org/wiki/Group_(periodic_table)"/>
-    <hyperlink ref="F1" r:id="rId4" tooltip="Period (periodic table)" display="https://en.wikipedia.org/wiki/Period_(periodic_table)"/>
-    <hyperlink ref="C2" r:id="rId5" tooltip="Hydrogen" display="https://en.wikipedia.org/wiki/Hydrogen"/>
-    <hyperlink ref="D2" r:id="rId6" tooltip="Greek language" display="https://en.wikipedia.org/wiki/Greek_language"/>
-    <hyperlink ref="C3" r:id="rId7" tooltip="Helium" display="https://en.wikipedia.org/wiki/Helium"/>
-    <hyperlink ref="C4" r:id="rId8" tooltip="Lithium" display="https://en.wikipedia.org/wiki/Lithium"/>
-    <hyperlink ref="C5" r:id="rId9" tooltip="Beryllium" display="https://en.wikipedia.org/wiki/Beryllium"/>
-    <hyperlink ref="D5" r:id="rId10" tooltip="Beryl" display="https://en.wikipedia.org/wiki/Beryl"/>
-    <hyperlink ref="C6" r:id="rId11" tooltip="Boron" display="https://en.wikipedia.org/wiki/Boron"/>
-    <hyperlink ref="D6" r:id="rId12" tooltip="Borax" display="https://en.wikipedia.org/wiki/Borax"/>
-    <hyperlink ref="C7" r:id="rId13" tooltip="Carbon" display="https://en.wikipedia.org/wiki/Carbon"/>
-    <hyperlink ref="D7" r:id="rId14" tooltip="Latin" display="https://en.wikipedia.org/wiki/Latin"/>
-    <hyperlink ref="C8" r:id="rId15" tooltip="Nitrogen" display="https://en.wikipedia.org/wiki/Nitrogen"/>
-    <hyperlink ref="D8" r:id="rId16" tooltip="Niter" display="https://en.wikipedia.org/wiki/Niter"/>
-    <hyperlink ref="C9" r:id="rId17" tooltip="Oxygen" display="https://en.wikipedia.org/wiki/Oxygen"/>
-    <hyperlink ref="C10" r:id="rId18" tooltip="Fluorine" display="https://en.wikipedia.org/wiki/Fluorine"/>
-    <hyperlink ref="C11" r:id="rId19" tooltip="Neon" display="https://en.wikipedia.org/wiki/Neon"/>
-    <hyperlink ref="C12" r:id="rId20" tooltip="Sodium" display="https://en.wikipedia.org/wiki/Sodium"/>
-    <hyperlink ref="D12" r:id="rId21" tooltip="English language" display="https://en.wikipedia.org/wiki/English_language"/>
-    <hyperlink ref="C13" r:id="rId22" tooltip="Magnesium" display="https://en.wikipedia.org/wiki/Magnesium"/>
-    <hyperlink ref="C14" r:id="rId23" tooltip="Aluminium" display="https://en.wikipedia.org/wiki/Aluminium"/>
-    <hyperlink ref="D14" r:id="rId24" tooltip="Aluminium oxide" display="https://en.wikipedia.org/wiki/Aluminium_oxide"/>
-    <hyperlink ref="C15" r:id="rId25" tooltip="Silicon" display="https://en.wikipedia.org/wiki/Silicon"/>
-    <hyperlink ref="C16" r:id="rId26" tooltip="Phosphorus" display="https://en.wikipedia.org/wiki/Phosphorus"/>
-    <hyperlink ref="C17" r:id="rId27" tooltip="Sulfur" display="https://en.wikipedia.org/wiki/Sulfur"/>
-    <hyperlink ref="C18" r:id="rId28" tooltip="Chlorine" display="https://en.wikipedia.org/wiki/Chlorine"/>
-    <hyperlink ref="C19" r:id="rId29" tooltip="Argon" display="https://en.wikipedia.org/wiki/Argon"/>
-    <hyperlink ref="C20" r:id="rId30" tooltip="Potassium" display="https://en.wikipedia.org/wiki/Potassium"/>
-    <hyperlink ref="D20" r:id="rId31" tooltip="New Latin" display="https://en.wikipedia.org/wiki/New_Latin"/>
-    <hyperlink ref="C21" r:id="rId32" tooltip="Calcium" display="https://en.wikipedia.org/wiki/Calcium"/>
-    <hyperlink ref="C22" r:id="rId33" tooltip="Scandium" display="https://en.wikipedia.org/wiki/Scandium"/>
-    <hyperlink ref="D22" r:id="rId34" tooltip="Scandinavia" display="https://en.wikipedia.org/wiki/Scandinavia"/>
-    <hyperlink ref="C23" r:id="rId35" tooltip="Titanium" display="https://en.wikipedia.org/wiki/Titanium"/>
-    <hyperlink ref="D23" r:id="rId36" tooltip="Titan (mythology)" display="https://en.wikipedia.org/wiki/Titan_(mythology)"/>
-    <hyperlink ref="C24" r:id="rId37" tooltip="Vanadium" display="https://en.wikipedia.org/wiki/Vanadium"/>
-    <hyperlink ref="C25" r:id="rId38" tooltip="Chromium" display="https://en.wikipedia.org/wiki/Chromium"/>
-    <hyperlink ref="C26" r:id="rId39" tooltip="Manganese" display="https://en.wikipedia.org/wiki/Manganese"/>
-    <hyperlink ref="C27" r:id="rId40" tooltip="Iron" display="https://en.wikipedia.org/wiki/Iron"/>
-    <hyperlink ref="C28" r:id="rId41" tooltip="Cobalt" display="https://en.wikipedia.org/wiki/Cobalt"/>
-    <hyperlink ref="D28" r:id="rId42" tooltip="German language" display="https://en.wikipedia.org/wiki/German_language"/>
-    <hyperlink ref="C29" r:id="rId43" tooltip="Nickel" display="https://en.wikipedia.org/wiki/Nickel"/>
-    <hyperlink ref="C30" r:id="rId44" tooltip="Copper" display="https://en.wikipedia.org/wiki/Copper"/>
-    <hyperlink ref="C31" r:id="rId45" tooltip="Zinc" display="https://en.wikipedia.org/wiki/Zinc"/>
-    <hyperlink ref="C32" r:id="rId46" tooltip="Gallium" display="https://en.wikipedia.org/wiki/Gallium"/>
-    <hyperlink ref="D32" r:id="rId47" tooltip="France" display="https://en.wikipedia.org/wiki/France"/>
-    <hyperlink ref="C33" r:id="rId48" tooltip="Germanium" display="https://en.wikipedia.org/wiki/Germanium"/>
-    <hyperlink ref="D33" r:id="rId49" tooltip="Germany" display="https://en.wikipedia.org/wiki/Germany"/>
-    <hyperlink ref="C34" r:id="rId50" tooltip="Arsenic" display="https://en.wikipedia.org/wiki/Arsenic"/>
-    <hyperlink ref="C35" r:id="rId51" tooltip="Selenium" display="https://en.wikipedia.org/wiki/Selenium"/>
-    <hyperlink ref="C36" r:id="rId52" tooltip="Bromine" display="https://en.wikipedia.org/wiki/Bromine"/>
-    <hyperlink ref="C37" r:id="rId53" tooltip="Krypton" display="https://en.wikipedia.org/wiki/Krypton"/>
-    <hyperlink ref="C38" r:id="rId54" tooltip="Rubidium" display="https://en.wikipedia.org/wiki/Rubidium"/>
-    <hyperlink ref="C39" r:id="rId55" tooltip="Strontium" display="https://en.wikipedia.org/wiki/Strontium"/>
-    <hyperlink ref="C40" r:id="rId56" tooltip="Yttrium" display="https://en.wikipedia.org/wiki/Yttrium"/>
-    <hyperlink ref="C41" r:id="rId57" tooltip="Zirconium" display="https://en.wikipedia.org/wiki/Zirconium"/>
-    <hyperlink ref="D41" r:id="rId58" tooltip="Jargoon" display="https://en.wikipedia.org/wiki/Jargoon"/>
-    <hyperlink ref="C42" r:id="rId59" tooltip="Niobium" display="https://en.wikipedia.org/wiki/Niobium"/>
-    <hyperlink ref="C43" r:id="rId60" tooltip="Molybdenum" display="https://en.wikipedia.org/wiki/Molybdenum"/>
-    <hyperlink ref="C44" r:id="rId61" tooltip="Technetium" display="https://en.wikipedia.org/wiki/Technetium"/>
-    <hyperlink ref="C45" r:id="rId62" tooltip="Ruthenium" display="https://en.wikipedia.org/wiki/Ruthenium"/>
-    <hyperlink ref="C46" r:id="rId63" tooltip="Rhodium" display="https://en.wikipedia.org/wiki/Rhodium"/>
-    <hyperlink ref="C47" r:id="rId64" tooltip="Palladium" display="https://en.wikipedia.org/wiki/Palladium"/>
-    <hyperlink ref="D47" r:id="rId65" tooltip="2 Pallas" display="https://en.wikipedia.org/wiki/2_Pallas"/>
-    <hyperlink ref="C48" r:id="rId66" tooltip="Silver" display="https://en.wikipedia.org/wiki/Silver"/>
-    <hyperlink ref="C49" r:id="rId67" tooltip="Cadmium" display="https://en.wikipedia.org/wiki/Cadmium"/>
-    <hyperlink ref="C50" r:id="rId68" tooltip="Indium" display="https://en.wikipedia.org/wiki/Indium"/>
-    <hyperlink ref="D50" r:id="rId69" tooltip="Indigo" display="https://en.wikipedia.org/wiki/Indigo"/>
-    <hyperlink ref="C51" r:id="rId70" tooltip="Tin" display="https://en.wikipedia.org/wiki/Tin"/>
-    <hyperlink ref="C52" r:id="rId71" tooltip="Antimony" display="https://en.wikipedia.org/wiki/Antimony"/>
-    <hyperlink ref="C53" r:id="rId72" tooltip="Tellurium" display="https://en.wikipedia.org/wiki/Tellurium"/>
-    <hyperlink ref="C54" r:id="rId73" tooltip="Iodine" display="https://en.wikipedia.org/wiki/Iodine"/>
-    <hyperlink ref="C55" r:id="rId74" tooltip="Xenon" display="https://en.wikipedia.org/wiki/Xenon"/>
-    <hyperlink ref="C56" r:id="rId75" tooltip="Caesium" display="https://en.wikipedia.org/wiki/Caesium"/>
-    <hyperlink ref="C57" r:id="rId76" tooltip="Barium" display="https://en.wikipedia.org/wiki/Barium"/>
-    <hyperlink ref="C58" r:id="rId77" tooltip="Lanthanum" display="https://en.wikipedia.org/wiki/Lanthanum"/>
-    <hyperlink ref="C59" r:id="rId78" tooltip="Cerium" display="https://en.wikipedia.org/wiki/Cerium"/>
-    <hyperlink ref="D59" r:id="rId79" tooltip="Ceres (dwarf planet)" display="https://en.wikipedia.org/wiki/Ceres_(dwarf_planet)"/>
-    <hyperlink ref="C60" r:id="rId80" tooltip="Praseodymium" display="https://en.wikipedia.org/wiki/Praseodymium"/>
-    <hyperlink ref="C61" r:id="rId81" tooltip="Neodymium" display="https://en.wikipedia.org/wiki/Neodymium"/>
-    <hyperlink ref="C62" r:id="rId82" tooltip="Promethium" display="https://en.wikipedia.org/wiki/Promethium"/>
-    <hyperlink ref="D62" r:id="rId83" tooltip="Prometheus" display="https://en.wikipedia.org/wiki/Prometheus"/>
-    <hyperlink ref="C63" r:id="rId84" tooltip="Samarium" display="https://en.wikipedia.org/wiki/Samarium"/>
-    <hyperlink ref="D63" r:id="rId85" tooltip="Samarskite" display="https://en.wikipedia.org/wiki/Samarskite"/>
-    <hyperlink ref="C64" r:id="rId86" tooltip="Europium" display="https://en.wikipedia.org/wiki/Europium"/>
-    <hyperlink ref="D64" r:id="rId87" tooltip="Europe" display="https://en.wikipedia.org/wiki/Europe"/>
-    <hyperlink ref="C65" r:id="rId88" tooltip="Gadolinium" display="https://en.wikipedia.org/wiki/Gadolinium"/>
-    <hyperlink ref="D65" r:id="rId89" tooltip="Johan Gadolin" display="https://en.wikipedia.org/wiki/Johan_Gadolin"/>
-    <hyperlink ref="C66" r:id="rId90" tooltip="Terbium" display="https://en.wikipedia.org/wiki/Terbium"/>
-    <hyperlink ref="D66" r:id="rId91" tooltip="Ytterby" display="https://en.wikipedia.org/wiki/Ytterby"/>
-    <hyperlink ref="C67" r:id="rId92" tooltip="Dysprosium" display="https://en.wikipedia.org/wiki/Dysprosium"/>
-    <hyperlink ref="C68" r:id="rId93" tooltip="Holmium" display="https://en.wikipedia.org/wiki/Holmium"/>
-    <hyperlink ref="C69" r:id="rId94" tooltip="Erbium" display="https://en.wikipedia.org/wiki/Erbium"/>
-    <hyperlink ref="D69" r:id="rId95" tooltip="Ytterby" display="https://en.wikipedia.org/wiki/Ytterby"/>
-    <hyperlink ref="C70" r:id="rId96" tooltip="Thulium" display="https://en.wikipedia.org/wiki/Thulium"/>
-    <hyperlink ref="D70" r:id="rId97" tooltip="Thule" display="https://en.wikipedia.org/wiki/Thule"/>
-    <hyperlink ref="C71" r:id="rId98" tooltip="Ytterbium" display="https://en.wikipedia.org/wiki/Ytterbium"/>
-    <hyperlink ref="D71" r:id="rId99" tooltip="Ytterby" display="https://en.wikipedia.org/wiki/Ytterby"/>
-    <hyperlink ref="C72" r:id="rId100" tooltip="Lutetium" display="https://en.wikipedia.org/wiki/Lutetium"/>
-    <hyperlink ref="D72" r:id="rId101" tooltip="Paris" display="https://en.wikipedia.org/wiki/Paris"/>
-    <hyperlink ref="C73" r:id="rId102" tooltip="Hafnium" display="https://en.wikipedia.org/wiki/Hafnium"/>
-    <hyperlink ref="D73" r:id="rId103" tooltip="Copenhagen" display="https://en.wikipedia.org/wiki/Copenhagen"/>
-    <hyperlink ref="C74" r:id="rId104" tooltip="Tantalum" display="https://en.wikipedia.org/wiki/Tantalum"/>
-    <hyperlink ref="D74" r:id="rId105" tooltip="Tantalus" display="https://en.wikipedia.org/wiki/Tantalus"/>
-    <hyperlink ref="C75" r:id="rId106" tooltip="Tungsten" display="https://en.wikipedia.org/wiki/Tungsten"/>
-    <hyperlink ref="C76" r:id="rId107" tooltip="Rhenium" display="https://en.wikipedia.org/wiki/Rhenium"/>
-    <hyperlink ref="D76" r:id="rId108" tooltip="Rhine" display="https://en.wikipedia.org/wiki/Rhine"/>
-    <hyperlink ref="C77" r:id="rId109" tooltip="Osmium" display="https://en.wikipedia.org/wiki/Osmium"/>
-    <hyperlink ref="C78" r:id="rId110" tooltip="Iridium" display="https://en.wikipedia.org/wiki/Iridium"/>
-    <hyperlink ref="D78" r:id="rId111" tooltip="Iris (mythology)" display="https://en.wikipedia.org/wiki/Iris_(mythology)"/>
-    <hyperlink ref="C79" r:id="rId112" tooltip="Platinum" display="https://en.wikipedia.org/wiki/Platinum"/>
-    <hyperlink ref="D79" r:id="rId113" tooltip="Spanish language" display="https://en.wikipedia.org/wiki/Spanish_language"/>
-    <hyperlink ref="C80" r:id="rId114" tooltip="Gold" display="https://en.wikipedia.org/wiki/Gold"/>
-    <hyperlink ref="C81" r:id="rId115" tooltip="Mercury (element)" display="https://en.wikipedia.org/wiki/Mercury_(element)"/>
-    <hyperlink ref="C82" r:id="rId116" tooltip="Thallium" display="https://en.wikipedia.org/wiki/Thallium"/>
-    <hyperlink ref="C83" r:id="rId117" tooltip="Lead" display="https://en.wikipedia.org/wiki/Lead"/>
-    <hyperlink ref="C84" r:id="rId118" tooltip="Bismuth" display="https://en.wikipedia.org/wiki/Bismuth"/>
-    <hyperlink ref="C85" r:id="rId119" tooltip="Polonium" display="https://en.wikipedia.org/wiki/Polonium"/>
-    <hyperlink ref="C86" r:id="rId120" tooltip="Astatine" display="https://en.wikipedia.org/wiki/Astatine"/>
-    <hyperlink ref="C87" r:id="rId121" tooltip="Radon" display="https://en.wikipedia.org/wiki/Radon"/>
-    <hyperlink ref="C88" r:id="rId122" tooltip="Francium" display="https://en.wikipedia.org/wiki/Francium"/>
-    <hyperlink ref="C89" r:id="rId123" tooltip="Radium" display="https://en.wikipedia.org/wiki/Radium"/>
-    <hyperlink ref="C90" r:id="rId124" tooltip="Actinium" display="https://en.wikipedia.org/wiki/Actinium"/>
-    <hyperlink ref="C91" r:id="rId125" tooltip="Thorium" display="https://en.wikipedia.org/wiki/Thorium"/>
-    <hyperlink ref="D91" r:id="rId126" tooltip="Thor" display="https://en.wikipedia.org/wiki/Thor"/>
-    <hyperlink ref="C92" r:id="rId127" tooltip="Protactinium" display="https://en.wikipedia.org/wiki/Protactinium"/>
-    <hyperlink ref="D92" r:id="rId128" tooltip="Actinium" display="https://en.wikipedia.org/wiki/Actinium"/>
-    <hyperlink ref="C93" r:id="rId129" tooltip="Uranium" display="https://en.wikipedia.org/wiki/Uranium"/>
-    <hyperlink ref="D93" r:id="rId130" tooltip="Uranus" display="https://en.wikipedia.org/wiki/Uranus"/>
-    <hyperlink ref="C94" r:id="rId131" tooltip="Neptunium" display="https://en.wikipedia.org/wiki/Neptunium"/>
-    <hyperlink ref="D94" r:id="rId132" tooltip="Neptune" display="https://en.wikipedia.org/wiki/Neptune"/>
-    <hyperlink ref="C95" r:id="rId133" tooltip="Plutonium" display="https://en.wikipedia.org/wiki/Plutonium"/>
-    <hyperlink ref="D95" r:id="rId134" tooltip="Pluto" display="https://en.wikipedia.org/wiki/Pluto"/>
-    <hyperlink ref="C96" r:id="rId135" tooltip="Americium" display="https://en.wikipedia.org/wiki/Americium"/>
-    <hyperlink ref="D96" r:id="rId136" tooltip="The Americas" display="https://en.wikipedia.org/wiki/The_Americas"/>
-    <hyperlink ref="C97" r:id="rId137" tooltip="Curium" display="https://en.wikipedia.org/wiki/Curium"/>
-    <hyperlink ref="C98" r:id="rId138" tooltip="Berkelium" display="https://en.wikipedia.org/wiki/Berkelium"/>
-    <hyperlink ref="D98" r:id="rId139" tooltip="Berkeley, California" display="https://en.wikipedia.org/wiki/Berkeley,_California"/>
-    <hyperlink ref="C99" r:id="rId140" tooltip="Californium" display="https://en.wikipedia.org/wiki/Californium"/>
-    <hyperlink ref="D99" r:id="rId141" tooltip="State of California" display="https://en.wikipedia.org/wiki/State_of_California"/>
-    <hyperlink ref="C100" r:id="rId142" tooltip="Einsteinium" display="https://en.wikipedia.org/wiki/Einsteinium"/>
-    <hyperlink ref="D100" r:id="rId143" tooltip="Albert Einstein" display="https://en.wikipedia.org/wiki/Albert_Einstein"/>
-    <hyperlink ref="C101" r:id="rId144" tooltip="Fermium" display="https://en.wikipedia.org/wiki/Fermium"/>
-    <hyperlink ref="D101" r:id="rId145" tooltip="Enrico Fermi" display="https://en.wikipedia.org/wiki/Enrico_Fermi"/>
-    <hyperlink ref="C102" r:id="rId146" tooltip="Mendelevium" display="https://en.wikipedia.org/wiki/Mendelevium"/>
-    <hyperlink ref="D102" r:id="rId147" tooltip="Dmitri Mendeleev" display="https://en.wikipedia.org/wiki/Dmitri_Mendeleev"/>
-    <hyperlink ref="C103" r:id="rId148" tooltip="Nobelium" display="https://en.wikipedia.org/wiki/Nobelium"/>
-    <hyperlink ref="D103" r:id="rId149" tooltip="Alfred Nobel" display="https://en.wikipedia.org/wiki/Alfred_Nobel"/>
-    <hyperlink ref="C104" r:id="rId150" tooltip="Lawrencium" display="https://en.wikipedia.org/wiki/Lawrencium"/>
-    <hyperlink ref="D104" r:id="rId151" tooltip="Ernest O. Lawrence" display="https://en.wikipedia.org/wiki/Ernest_O._Lawrence"/>
-    <hyperlink ref="C105" r:id="rId152" tooltip="Rutherfordium" display="https://en.wikipedia.org/wiki/Rutherfordium"/>
-    <hyperlink ref="D105" r:id="rId153" tooltip="Ernest Rutherford" display="https://en.wikipedia.org/wiki/Ernest_Rutherford"/>
-    <hyperlink ref="C106" r:id="rId154" tooltip="Dubnium" display="https://en.wikipedia.org/wiki/Dubnium"/>
-    <hyperlink ref="D106" r:id="rId155" tooltip="Dubna" display="https://en.wikipedia.org/wiki/Dubna"/>
-    <hyperlink ref="C107" r:id="rId156" tooltip="Seaborgium" display="https://en.wikipedia.org/wiki/Seaborgium"/>
-    <hyperlink ref="D107" r:id="rId157" tooltip="Glenn T. Seaborg" display="https://en.wikipedia.org/wiki/Glenn_T._Seaborg"/>
-    <hyperlink ref="C108" r:id="rId158" tooltip="Bohrium" display="https://en.wikipedia.org/wiki/Bohrium"/>
-    <hyperlink ref="D108" r:id="rId159" tooltip="Niels Bohr" display="https://en.wikipedia.org/wiki/Niels_Bohr"/>
-    <hyperlink ref="C109" r:id="rId160" tooltip="Hassium" display="https://en.wikipedia.org/wiki/Hassium"/>
-    <hyperlink ref="D109" r:id="rId161" tooltip="Hesse" display="https://en.wikipedia.org/wiki/Hesse"/>
-    <hyperlink ref="C110" r:id="rId162" tooltip="Meitnerium" display="https://en.wikipedia.org/wiki/Meitnerium"/>
-    <hyperlink ref="D110" r:id="rId163" tooltip="Lise Meitner" display="https://en.wikipedia.org/wiki/Lise_Meitner"/>
-    <hyperlink ref="C111" r:id="rId164" tooltip="Darmstadtium" display="https://en.wikipedia.org/wiki/Darmstadtium"/>
-    <hyperlink ref="D111" r:id="rId165" tooltip="Darmstadt" display="https://en.wikipedia.org/wiki/Darmstadt"/>
-    <hyperlink ref="C112" r:id="rId166" tooltip="Roentgenium" display="https://en.wikipedia.org/wiki/Roentgenium"/>
-    <hyperlink ref="D112" r:id="rId167" tooltip="Wilhelm Conrad Röntgen" display="https://en.wikipedia.org/wiki/Wilhelm_Conrad_R%C3%B6ntgen"/>
-    <hyperlink ref="C113" r:id="rId168" tooltip="Copernicium" display="https://en.wikipedia.org/wiki/Copernicium"/>
-    <hyperlink ref="D113" r:id="rId169" tooltip="Nicolaus Copernicus" display="https://en.wikipedia.org/wiki/Nicolaus_Copernicus"/>
-    <hyperlink ref="C114" r:id="rId170" tooltip="Nihonium" display="https://en.wikipedia.org/wiki/Nihonium"/>
-    <hyperlink ref="C115" r:id="rId171" tooltip="Flerovium" display="https://en.wikipedia.org/wiki/Flerovium"/>
-    <hyperlink ref="C116" r:id="rId172" tooltip="Moscovium" display="https://en.wikipedia.org/wiki/Moscovium"/>
-    <hyperlink ref="D116" r:id="rId173" tooltip="Moscow Oblast" display="https://en.wikipedia.org/wiki/Moscow_Oblast"/>
-    <hyperlink ref="C117" r:id="rId174" tooltip="Livermorium" display="https://en.wikipedia.org/wiki/Livermorium"/>
-    <hyperlink ref="C118" r:id="rId175" tooltip="Tennessine" display="https://en.wikipedia.org/wiki/Tennessine"/>
-    <hyperlink ref="D118" r:id="rId176" tooltip="Tennessee" display="https://en.wikipedia.org/wiki/Tennessee"/>
-    <hyperlink ref="C119" r:id="rId177" tooltip="Oganesson" display="https://en.wikipedia.org/wiki/Oganesson"/>
-    <hyperlink ref="D119" r:id="rId178" tooltip="Yuri Oganessian" display="https://en.wikipedia.org/wiki/Yuri_Oganessian"/>
+    <hyperlink ref="B1" r:id="rId1" tooltip="Symbol (chemistry)" display="https://en.wikipedia.org/wiki/Symbol_(chemistry)" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C1" r:id="rId2" tooltip="Chemical element" display="https://en.wikipedia.org/wiki/Chemical_element" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E1" r:id="rId3" tooltip="Group (periodic table)" display="https://en.wikipedia.org/wiki/Group_(periodic_table)" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F1" r:id="rId4" tooltip="Period (periodic table)" display="https://en.wikipedia.org/wiki/Period_(periodic_table)" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" tooltip="Hydrogen" display="https://en.wikipedia.org/wiki/Hydrogen" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId6" tooltip="Greek language" display="https://en.wikipedia.org/wiki/Greek_language" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C3" r:id="rId7" tooltip="Helium" display="https://en.wikipedia.org/wiki/Helium" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C4" r:id="rId8" tooltip="Lithium" display="https://en.wikipedia.org/wiki/Lithium" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C5" r:id="rId9" tooltip="Beryllium" display="https://en.wikipedia.org/wiki/Beryllium" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D5" r:id="rId10" tooltip="Beryl" display="https://en.wikipedia.org/wiki/Beryl" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C6" r:id="rId11" tooltip="Boron" display="https://en.wikipedia.org/wiki/Boron" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D6" r:id="rId12" tooltip="Borax" display="https://en.wikipedia.org/wiki/Borax" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C7" r:id="rId13" tooltip="Carbon" display="https://en.wikipedia.org/wiki/Carbon" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D7" r:id="rId14" tooltip="Latin" display="https://en.wikipedia.org/wiki/Latin" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C8" r:id="rId15" tooltip="Nitrogen" display="https://en.wikipedia.org/wiki/Nitrogen" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D8" r:id="rId16" tooltip="Niter" display="https://en.wikipedia.org/wiki/Niter" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C9" r:id="rId17" tooltip="Oxygen" display="https://en.wikipedia.org/wiki/Oxygen" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C10" r:id="rId18" tooltip="Fluorine" display="https://en.wikipedia.org/wiki/Fluorine" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C11" r:id="rId19" tooltip="Neon" display="https://en.wikipedia.org/wiki/Neon" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C12" r:id="rId20" tooltip="Sodium" display="https://en.wikipedia.org/wiki/Sodium" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D12" r:id="rId21" tooltip="English language" display="https://en.wikipedia.org/wiki/English_language" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C13" r:id="rId22" tooltip="Magnesium" display="https://en.wikipedia.org/wiki/Magnesium" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C14" r:id="rId23" tooltip="Aluminium" display="https://en.wikipedia.org/wiki/Aluminium" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D14" r:id="rId24" tooltip="Aluminium oxide" display="https://en.wikipedia.org/wiki/Aluminium_oxide" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C15" r:id="rId25" tooltip="Silicon" display="https://en.wikipedia.org/wiki/Silicon" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C16" r:id="rId26" tooltip="Phosphorus" display="https://en.wikipedia.org/wiki/Phosphorus" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C17" r:id="rId27" tooltip="Sulfur" display="https://en.wikipedia.org/wiki/Sulfur" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C18" r:id="rId28" tooltip="Chlorine" display="https://en.wikipedia.org/wiki/Chlorine" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C19" r:id="rId29" tooltip="Argon" display="https://en.wikipedia.org/wiki/Argon" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C20" r:id="rId30" tooltip="Potassium" display="https://en.wikipedia.org/wiki/Potassium" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D20" r:id="rId31" tooltip="New Latin" display="https://en.wikipedia.org/wiki/New_Latin" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C21" r:id="rId32" tooltip="Calcium" display="https://en.wikipedia.org/wiki/Calcium" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C22" r:id="rId33" tooltip="Scandium" display="https://en.wikipedia.org/wiki/Scandium" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D22" r:id="rId34" tooltip="Scandinavia" display="https://en.wikipedia.org/wiki/Scandinavia" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C23" r:id="rId35" tooltip="Titanium" display="https://en.wikipedia.org/wiki/Titanium" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D23" r:id="rId36" tooltip="Titan (mythology)" display="https://en.wikipedia.org/wiki/Titan_(mythology)" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C24" r:id="rId37" tooltip="Vanadium" display="https://en.wikipedia.org/wiki/Vanadium" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C25" r:id="rId38" tooltip="Chromium" display="https://en.wikipedia.org/wiki/Chromium" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C26" r:id="rId39" tooltip="Manganese" display="https://en.wikipedia.org/wiki/Manganese" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C27" r:id="rId40" tooltip="Iron" display="https://en.wikipedia.org/wiki/Iron" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C28" r:id="rId41" tooltip="Cobalt" display="https://en.wikipedia.org/wiki/Cobalt" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D28" r:id="rId42" tooltip="German language" display="https://en.wikipedia.org/wiki/German_language" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C29" r:id="rId43" tooltip="Nickel" display="https://en.wikipedia.org/wiki/Nickel" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C30" r:id="rId44" tooltip="Copper" display="https://en.wikipedia.org/wiki/Copper" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C31" r:id="rId45" tooltip="Zinc" display="https://en.wikipedia.org/wiki/Zinc" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C32" r:id="rId46" tooltip="Gallium" display="https://en.wikipedia.org/wiki/Gallium" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D32" r:id="rId47" tooltip="France" display="https://en.wikipedia.org/wiki/France" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C33" r:id="rId48" tooltip="Germanium" display="https://en.wikipedia.org/wiki/Germanium" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D33" r:id="rId49" tooltip="Germany" display="https://en.wikipedia.org/wiki/Germany" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C34" r:id="rId50" tooltip="Arsenic" display="https://en.wikipedia.org/wiki/Arsenic" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C35" r:id="rId51" tooltip="Selenium" display="https://en.wikipedia.org/wiki/Selenium" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C36" r:id="rId52" tooltip="Bromine" display="https://en.wikipedia.org/wiki/Bromine" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C37" r:id="rId53" tooltip="Krypton" display="https://en.wikipedia.org/wiki/Krypton" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C38" r:id="rId54" tooltip="Rubidium" display="https://en.wikipedia.org/wiki/Rubidium" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C39" r:id="rId55" tooltip="Strontium" display="https://en.wikipedia.org/wiki/Strontium" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C40" r:id="rId56" tooltip="Yttrium" display="https://en.wikipedia.org/wiki/Yttrium" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C41" r:id="rId57" tooltip="Zirconium" display="https://en.wikipedia.org/wiki/Zirconium" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="D41" r:id="rId58" tooltip="Jargoon" display="https://en.wikipedia.org/wiki/Jargoon" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C42" r:id="rId59" tooltip="Niobium" display="https://en.wikipedia.org/wiki/Niobium" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C43" r:id="rId60" tooltip="Molybdenum" display="https://en.wikipedia.org/wiki/Molybdenum" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C44" r:id="rId61" tooltip="Technetium" display="https://en.wikipedia.org/wiki/Technetium" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C45" r:id="rId62" tooltip="Ruthenium" display="https://en.wikipedia.org/wiki/Ruthenium" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C46" r:id="rId63" tooltip="Rhodium" display="https://en.wikipedia.org/wiki/Rhodium" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C47" r:id="rId64" tooltip="Palladium" display="https://en.wikipedia.org/wiki/Palladium" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="D47" r:id="rId65" tooltip="2 Pallas" display="https://en.wikipedia.org/wiki/2_Pallas" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C48" r:id="rId66" tooltip="Silver" display="https://en.wikipedia.org/wiki/Silver" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C49" r:id="rId67" tooltip="Cadmium" display="https://en.wikipedia.org/wiki/Cadmium" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C50" r:id="rId68" tooltip="Indium" display="https://en.wikipedia.org/wiki/Indium" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D50" r:id="rId69" tooltip="Indigo" display="https://en.wikipedia.org/wiki/Indigo" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C51" r:id="rId70" tooltip="Tin" display="https://en.wikipedia.org/wiki/Tin" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C52" r:id="rId71" tooltip="Antimony" display="https://en.wikipedia.org/wiki/Antimony" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="C53" r:id="rId72" tooltip="Tellurium" display="https://en.wikipedia.org/wiki/Tellurium" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C54" r:id="rId73" tooltip="Iodine" display="https://en.wikipedia.org/wiki/Iodine" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="C55" r:id="rId74" tooltip="Xenon" display="https://en.wikipedia.org/wiki/Xenon" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C56" r:id="rId75" tooltip="Caesium" display="https://en.wikipedia.org/wiki/Caesium" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C57" r:id="rId76" tooltip="Barium" display="https://en.wikipedia.org/wiki/Barium" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C58" r:id="rId77" tooltip="Lanthanum" display="https://en.wikipedia.org/wiki/Lanthanum" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C59" r:id="rId78" tooltip="Cerium" display="https://en.wikipedia.org/wiki/Cerium" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="D59" r:id="rId79" tooltip="Ceres (dwarf planet)" display="https://en.wikipedia.org/wiki/Ceres_(dwarf_planet)" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="C60" r:id="rId80" tooltip="Praseodymium" display="https://en.wikipedia.org/wiki/Praseodymium" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C61" r:id="rId81" tooltip="Neodymium" display="https://en.wikipedia.org/wiki/Neodymium" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="C62" r:id="rId82" tooltip="Promethium" display="https://en.wikipedia.org/wiki/Promethium" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="D62" r:id="rId83" tooltip="Prometheus" display="https://en.wikipedia.org/wiki/Prometheus" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="C63" r:id="rId84" tooltip="Samarium" display="https://en.wikipedia.org/wiki/Samarium" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="D63" r:id="rId85" tooltip="Samarskite" display="https://en.wikipedia.org/wiki/Samarskite" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C64" r:id="rId86" tooltip="Europium" display="https://en.wikipedia.org/wiki/Europium" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="D64" r:id="rId87" tooltip="Europe" display="https://en.wikipedia.org/wiki/Europe" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="C65" r:id="rId88" tooltip="Gadolinium" display="https://en.wikipedia.org/wiki/Gadolinium" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="D65" r:id="rId89" tooltip="Johan Gadolin" display="https://en.wikipedia.org/wiki/Johan_Gadolin" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C66" r:id="rId90" tooltip="Terbium" display="https://en.wikipedia.org/wiki/Terbium" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="D66" r:id="rId91" tooltip="Ytterby" display="https://en.wikipedia.org/wiki/Ytterby" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="C67" r:id="rId92" tooltip="Dysprosium" display="https://en.wikipedia.org/wiki/Dysprosium" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="C68" r:id="rId93" tooltip="Holmium" display="https://en.wikipedia.org/wiki/Holmium" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="C69" r:id="rId94" tooltip="Erbium" display="https://en.wikipedia.org/wiki/Erbium" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="D69" r:id="rId95" tooltip="Ytterby" display="https://en.wikipedia.org/wiki/Ytterby" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="C70" r:id="rId96" tooltip="Thulium" display="https://en.wikipedia.org/wiki/Thulium" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="D70" r:id="rId97" tooltip="Thule" display="https://en.wikipedia.org/wiki/Thule" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="C71" r:id="rId98" tooltip="Ytterbium" display="https://en.wikipedia.org/wiki/Ytterbium" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="D71" r:id="rId99" tooltip="Ytterby" display="https://en.wikipedia.org/wiki/Ytterby" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="C72" r:id="rId100" tooltip="Lutetium" display="https://en.wikipedia.org/wiki/Lutetium" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D72" r:id="rId101" tooltip="Paris" display="https://en.wikipedia.org/wiki/Paris" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C73" r:id="rId102" tooltip="Hafnium" display="https://en.wikipedia.org/wiki/Hafnium" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="D73" r:id="rId103" tooltip="Copenhagen" display="https://en.wikipedia.org/wiki/Copenhagen" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="C74" r:id="rId104" tooltip="Tantalum" display="https://en.wikipedia.org/wiki/Tantalum" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="D74" r:id="rId105" tooltip="Tantalus" display="https://en.wikipedia.org/wiki/Tantalus" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="C75" r:id="rId106" tooltip="Tungsten" display="https://en.wikipedia.org/wiki/Tungsten" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="C76" r:id="rId107" tooltip="Rhenium" display="https://en.wikipedia.org/wiki/Rhenium" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="D76" r:id="rId108" tooltip="Rhine" display="https://en.wikipedia.org/wiki/Rhine" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="C77" r:id="rId109" tooltip="Osmium" display="https://en.wikipedia.org/wiki/Osmium" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="C78" r:id="rId110" tooltip="Iridium" display="https://en.wikipedia.org/wiki/Iridium" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D78" r:id="rId111" tooltip="Iris (mythology)" display="https://en.wikipedia.org/wiki/Iris_(mythology)" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C79" r:id="rId112" tooltip="Platinum" display="https://en.wikipedia.org/wiki/Platinum" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="D79" r:id="rId113" tooltip="Spanish language" display="https://en.wikipedia.org/wiki/Spanish_language" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="C80" r:id="rId114" tooltip="Gold" display="https://en.wikipedia.org/wiki/Gold" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="C81" r:id="rId115" tooltip="Mercury (element)" display="https://en.wikipedia.org/wiki/Mercury_(element)" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="C82" r:id="rId116" tooltip="Thallium" display="https://en.wikipedia.org/wiki/Thallium" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="C83" r:id="rId117" tooltip="Lead" display="https://en.wikipedia.org/wiki/Lead" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="C84" r:id="rId118" tooltip="Bismuth" display="https://en.wikipedia.org/wiki/Bismuth" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="C85" r:id="rId119" tooltip="Polonium" display="https://en.wikipedia.org/wiki/Polonium" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="C86" r:id="rId120" tooltip="Astatine" display="https://en.wikipedia.org/wiki/Astatine" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="C87" r:id="rId121" tooltip="Radon" display="https://en.wikipedia.org/wiki/Radon" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="C88" r:id="rId122" tooltip="Francium" display="https://en.wikipedia.org/wiki/Francium" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="C89" r:id="rId123" tooltip="Radium" display="https://en.wikipedia.org/wiki/Radium" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="C90" r:id="rId124" tooltip="Actinium" display="https://en.wikipedia.org/wiki/Actinium" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="C91" r:id="rId125" tooltip="Thorium" display="https://en.wikipedia.org/wiki/Thorium" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="D91" r:id="rId126" tooltip="Thor" display="https://en.wikipedia.org/wiki/Thor" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="C92" r:id="rId127" tooltip="Protactinium" display="https://en.wikipedia.org/wiki/Protactinium" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="D92" r:id="rId128" tooltip="Actinium" display="https://en.wikipedia.org/wiki/Actinium" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="C93" r:id="rId129" tooltip="Uranium" display="https://en.wikipedia.org/wiki/Uranium" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="D93" r:id="rId130" tooltip="Uranus" display="https://en.wikipedia.org/wiki/Uranus" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="C94" r:id="rId131" tooltip="Neptunium" display="https://en.wikipedia.org/wiki/Neptunium" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="D94" r:id="rId132" tooltip="Neptune" display="https://en.wikipedia.org/wiki/Neptune" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="C95" r:id="rId133" tooltip="Plutonium" display="https://en.wikipedia.org/wiki/Plutonium" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="D95" r:id="rId134" tooltip="Pluto" display="https://en.wikipedia.org/wiki/Pluto" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="C96" r:id="rId135" tooltip="Americium" display="https://en.wikipedia.org/wiki/Americium" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="D96" r:id="rId136" tooltip="The Americas" display="https://en.wikipedia.org/wiki/The_Americas" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="C97" r:id="rId137" tooltip="Curium" display="https://en.wikipedia.org/wiki/Curium" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="C98" r:id="rId138" tooltip="Berkelium" display="https://en.wikipedia.org/wiki/Berkelium" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="D98" r:id="rId139" tooltip="Berkeley, California" display="https://en.wikipedia.org/wiki/Berkeley,_California" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="C99" r:id="rId140" tooltip="Californium" display="https://en.wikipedia.org/wiki/Californium" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="D99" r:id="rId141" tooltip="State of California" display="https://en.wikipedia.org/wiki/State_of_California" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="C100" r:id="rId142" tooltip="Einsteinium" display="https://en.wikipedia.org/wiki/Einsteinium" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="D100" r:id="rId143" tooltip="Albert Einstein" display="https://en.wikipedia.org/wiki/Albert_Einstein" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="C101" r:id="rId144" tooltip="Fermium" display="https://en.wikipedia.org/wiki/Fermium" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="D101" r:id="rId145" tooltip="Enrico Fermi" display="https://en.wikipedia.org/wiki/Enrico_Fermi" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="C102" r:id="rId146" tooltip="Mendelevium" display="https://en.wikipedia.org/wiki/Mendelevium" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="D102" r:id="rId147" tooltip="Dmitri Mendeleev" display="https://en.wikipedia.org/wiki/Dmitri_Mendeleev" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="C103" r:id="rId148" tooltip="Nobelium" display="https://en.wikipedia.org/wiki/Nobelium" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="D103" r:id="rId149" tooltip="Alfred Nobel" display="https://en.wikipedia.org/wiki/Alfred_Nobel" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="C104" r:id="rId150" tooltip="Lawrencium" display="https://en.wikipedia.org/wiki/Lawrencium" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="D104" r:id="rId151" tooltip="Ernest O. Lawrence" display="https://en.wikipedia.org/wiki/Ernest_O._Lawrence" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="C105" r:id="rId152" tooltip="Rutherfordium" display="https://en.wikipedia.org/wiki/Rutherfordium" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="D105" r:id="rId153" tooltip="Ernest Rutherford" display="https://en.wikipedia.org/wiki/Ernest_Rutherford" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="C106" r:id="rId154" tooltip="Dubnium" display="https://en.wikipedia.org/wiki/Dubnium" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="D106" r:id="rId155" tooltip="Dubna" display="https://en.wikipedia.org/wiki/Dubna" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="C107" r:id="rId156" tooltip="Seaborgium" display="https://en.wikipedia.org/wiki/Seaborgium" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="D107" r:id="rId157" tooltip="Glenn T. Seaborg" display="https://en.wikipedia.org/wiki/Glenn_T._Seaborg" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="C108" r:id="rId158" tooltip="Bohrium" display="https://en.wikipedia.org/wiki/Bohrium" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="D108" r:id="rId159" tooltip="Niels Bohr" display="https://en.wikipedia.org/wiki/Niels_Bohr" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="C109" r:id="rId160" tooltip="Hassium" display="https://en.wikipedia.org/wiki/Hassium" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="D109" r:id="rId161" tooltip="Hesse" display="https://en.wikipedia.org/wiki/Hesse" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="C110" r:id="rId162" tooltip="Meitnerium" display="https://en.wikipedia.org/wiki/Meitnerium" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="D110" r:id="rId163" tooltip="Lise Meitner" display="https://en.wikipedia.org/wiki/Lise_Meitner" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="C111" r:id="rId164" tooltip="Darmstadtium" display="https://en.wikipedia.org/wiki/Darmstadtium" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="D111" r:id="rId165" tooltip="Darmstadt" display="https://en.wikipedia.org/wiki/Darmstadt" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="C112" r:id="rId166" tooltip="Roentgenium" display="https://en.wikipedia.org/wiki/Roentgenium" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="D112" r:id="rId167" tooltip="Wilhelm Conrad Röntgen" display="https://en.wikipedia.org/wiki/Wilhelm_Conrad_R%C3%B6ntgen" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="C113" r:id="rId168" tooltip="Copernicium" display="https://en.wikipedia.org/wiki/Copernicium" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="D113" r:id="rId169" tooltip="Nicolaus Copernicus" display="https://en.wikipedia.org/wiki/Nicolaus_Copernicus" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="C114" r:id="rId170" tooltip="Nihonium" display="https://en.wikipedia.org/wiki/Nihonium" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="C115" r:id="rId171" tooltip="Flerovium" display="https://en.wikipedia.org/wiki/Flerovium" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="C116" r:id="rId172" tooltip="Moscovium" display="https://en.wikipedia.org/wiki/Moscovium" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="D116" r:id="rId173" tooltip="Moscow Oblast" display="https://en.wikipedia.org/wiki/Moscow_Oblast" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="C117" r:id="rId174" tooltip="Livermorium" display="https://en.wikipedia.org/wiki/Livermorium" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="C118" r:id="rId175" tooltip="Tennessine" display="https://en.wikipedia.org/wiki/Tennessine" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="D118" r:id="rId176" tooltip="Tennessee" display="https://en.wikipedia.org/wiki/Tennessee" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="C119" r:id="rId177" tooltip="Oganesson" display="https://en.wikipedia.org/wiki/Oganesson" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="D119" r:id="rId178" tooltip="Yuri Oganessian" display="https://en.wikipedia.org/wiki/Yuri_Oganessian" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId179"/>
@@ -6652,7 +6696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6664,7 +6708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>